<commit_message>
update rssi measurement test results
</commit_message>
<xml_diff>
--- a/results/rssi_measurement_results.xlsx
+++ b/results/rssi_measurement_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Clones\LPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\lps\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000AE20B-C6F5-4562-92C3-5ADBA1C486D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99892C43-46B6-4342-AD41-A1820693FE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2DCB29A0-4F39-4CA9-9859-1744B998AF1F}"/>
+    <workbookView xWindow="0" yWindow="390" windowWidth="29010" windowHeight="12855" xr2:uid="{2DCB29A0-4F39-4CA9-9859-1744B998AF1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t>Distance</t>
-  </si>
-  <si>
     <t>Room characteristics:</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>Measurements were assisted by directing the antenna</t>
+  </si>
+  <si>
+    <t>Distance in m</t>
   </si>
 </sst>
 </file>
@@ -291,19 +291,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -314,11 +309,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -658,35 +658,50 @@
   <dimension ref="A2:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -705,16 +720,16 @@
       <c r="F7" s="1">
         <v>5</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>-70</v>
@@ -731,476 +746,478 @@
       <c r="F8">
         <v>-75</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <f>AVERAGE(B8:F8)</f>
         <v>-70</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8">
         <f>MEDIAN(B8:F8)</f>
         <v>-70</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>-67</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>-68</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>-65</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>-67</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>-65</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="6">
         <f>AVERAGE(B9:F9)</f>
         <v>-66.400000000000006</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="4">
         <f>MEDIAN(B9:F9)</f>
         <v>-67</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="7">
+        <v>4</v>
+      </c>
+      <c r="B10">
         <v>-74</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10">
         <v>-73</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10">
         <v>-85</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10">
         <v>-74</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10">
         <v>-74</v>
       </c>
-      <c r="G10" s="6">
-        <f t="shared" ref="G10:G24" si="0">AVERAGE(B10:F10)</f>
+      <c r="G10" s="5">
+        <f t="shared" ref="G10" si="0">AVERAGE(B10:F10)</f>
         <v>-76</v>
       </c>
-      <c r="H10" s="7">
-        <f t="shared" ref="H10:H24" si="1">MEDIAN(B10:F10)</f>
+      <c r="H10">
+        <f t="shared" ref="H10" si="1">MEDIAN(B10:F10)</f>
         <v>-74</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="14">
+      <c r="B11" s="11">
         <v>-67</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="11">
         <v>-68</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="11">
         <v>-72</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="11">
         <v>-69</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="11">
         <v>-73</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="12">
         <f t="shared" ref="G11:G12" si="2">AVERAGE(B11:F11)</f>
         <v>-69.8</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="11">
         <f t="shared" ref="H11:H12" si="3">MEDIAN(B11:F11)</f>
         <v>-69</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="12">
+      <c r="A12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="9">
         <v>-77</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="9">
         <v>-76</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="9">
         <v>-82</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="9">
         <v>-76</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="9">
         <v>-77</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="10">
         <f t="shared" si="2"/>
         <v>-77.599999999999994</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="9">
         <f t="shared" si="3"/>
         <v>-77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="14">
+      <c r="B13" s="11">
         <v>-77</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="11">
         <v>-71</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="11">
         <v>-71</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="11">
         <v>-74</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="11">
         <v>-72</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="12">
         <f t="shared" ref="G13:G24" si="4">AVERAGE(B13:F13)</f>
         <v>-73</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="11">
         <f t="shared" ref="H13:H24" si="5">MEDIAN(B13:F13)</f>
         <v>-72</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="12">
+      <c r="A14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="9">
         <v>-90</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="9">
         <v>-85</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="9">
         <v>-83</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="9">
         <v>-89</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="9">
         <v>-87</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="10">
         <f t="shared" si="4"/>
         <v>-86.8</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="9">
         <f t="shared" si="5"/>
         <v>-87</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="14">
+      <c r="B15" s="11">
         <v>-83</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="11">
         <v>-81</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="11">
         <v>-79</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="11">
         <v>-78</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="11">
         <v>-76</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="12">
         <f t="shared" si="4"/>
         <v>-79.400000000000006</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="11">
         <f t="shared" si="5"/>
         <v>-79</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="12">
+      <c r="A16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="9">
         <v>-89</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="9">
         <v>-96</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="9">
         <v>-90</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="9">
         <v>-91</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="9">
         <v>-90</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="10">
         <f t="shared" si="4"/>
         <v>-91.2</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="9">
         <f t="shared" si="5"/>
         <v>-90</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="14">
+      <c r="B17" s="11">
         <v>-78</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="11">
         <v>-86</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="11">
         <v>-77</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="11">
         <v>-85</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="11">
         <v>-77</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="12">
         <f t="shared" si="4"/>
         <v>-80.599999999999994</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="11">
         <f t="shared" si="5"/>
         <v>-78</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="12">
+      <c r="A18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="9">
         <v>-92</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="9">
         <v>-94</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="9">
         <v>-88</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="9">
         <v>-98</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="9">
         <v>-92</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="10">
         <f t="shared" si="4"/>
         <v>-92.8</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="9">
         <f t="shared" si="5"/>
         <v>-92</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="14">
+      <c r="B19" s="11">
         <v>-94</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="11">
         <v>-85</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="11">
         <v>-89</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="11">
         <v>-85</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="11">
         <v>-95</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="12">
         <f t="shared" si="4"/>
         <v>-89.6</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="11">
         <f t="shared" si="5"/>
         <v>-89</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="12">
+      <c r="A20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="9">
         <v>-97</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="9">
         <v>-93</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="9">
         <v>-98</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="9">
         <v>-96</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="9">
         <v>-94</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="10">
         <f t="shared" si="4"/>
         <v>-95.6</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="9">
         <f t="shared" si="5"/>
         <v>-96</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="14">
+      <c r="B21" s="11">
         <v>-98</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="11">
         <v>-88</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="11">
         <v>-86</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="11">
         <v>-87</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="11">
         <v>-88</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="12">
         <f t="shared" si="4"/>
         <v>-89.4</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="11">
         <f t="shared" si="5"/>
         <v>-88</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="18">
+      <c r="A22" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="15">
         <v>-101</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="15">
         <v>-98</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="15">
         <v>-89</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="15">
         <v>-93</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="15">
         <v>-97</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="16">
         <f t="shared" si="4"/>
         <v>-95.6</v>
       </c>
-      <c r="H22" s="18">
+      <c r="H22" s="15">
         <f t="shared" si="5"/>
         <v>-97</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="18">
+      <c r="A23" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="15">
         <v>-95</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="15">
         <v>-96</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="15">
         <v>-96</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="15">
         <v>-95</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="15">
         <v>-95</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="16">
         <f t="shared" si="4"/>
         <v>-95.4</v>
       </c>
-      <c r="H23" s="18">
+      <c r="H23" s="15">
         <f t="shared" si="5"/>
         <v>-95</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="18">
+      <c r="A24" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="15">
         <v>-105</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="15">
         <v>-101</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="15">
         <v>-97</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="15">
         <v>-98</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="15">
         <v>-97</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="16">
         <f t="shared" si="4"/>
         <v>-99.6</v>
       </c>
-      <c r="H24" s="18">
+      <c r="H24" s="15">
         <f t="shared" si="5"/>
         <v>-98</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B26:H26"/>
     <mergeCell ref="B27:H27"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>